<commit_message>
Add columns to pass validation.
</commit_message>
<xml_diff>
--- a/test/fixtures/input/subjects.xlsx
+++ b/test/fixtures/input/subjects.xlsx
@@ -1,36 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/loneyf/workspace/immpload/test/fixtures/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A64E6A19-E639-4E4A-9C35-1243C3981CE5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="3800" yWindow="3620" windowWidth="20620" windowHeight="12860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weights" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>ID</t>
   </si>
@@ -72,12 +67,27 @@
   </si>
   <si>
     <t>n/a</t>
+  </si>
+  <si>
+    <t>Strain</t>
+  </si>
+  <si>
+    <t>8034x8043</t>
+  </si>
+  <si>
+    <t>15119x16521</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -395,110 +405,134 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.5" customWidth="1"/>
-    <col min="4" max="4" width="11" style="2"/>
+    <col min="1" max="2" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
+    <col min="5" max="5" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>42338</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <v>42338</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="1">
         <v>42338</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="1">
         <v>42338</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="1">
         <v>42338</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D7" s="1">
         <v>42338</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>